<commit_message>
Bug fixes and parse filters
</commit_message>
<xml_diff>
--- a/MappingConfigFile.xlsx
+++ b/MappingConfigFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fortran\eric\adp13b_1group_heatloss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AIPP3ScilabConvertCompare\GIT\AIPP_scilab_Convert_Compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A267A5-0809-49B1-8DFB-3CD02D8B9867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF0B4E9-3CC5-4FF1-AD22-0F79D42215CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="12630" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31875" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MappingTable" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="96">
   <si>
     <t>AIPP 2.3.5</t>
   </si>
@@ -104,21 +104,12 @@
     <t>Texit*</t>
   </si>
   <si>
-    <t>Exit_Temperature</t>
-  </si>
-  <si>
     <t>Twall*</t>
   </si>
   <si>
-    <t>Wall_Temperature</t>
-  </si>
-  <si>
     <t>Tpack*</t>
   </si>
   <si>
-    <t>Pack_Temperature</t>
-  </si>
-  <si>
     <t>Mdot</t>
   </si>
   <si>
@@ -131,81 +122,6 @@
     <t>Mass_Flow_To_Tank</t>
   </si>
   <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>Molecular_Weight</t>
-  </si>
-  <si>
-    <t>Cp</t>
-  </si>
-  <si>
-    <t>Cv</t>
-  </si>
-  <si>
-    <t>gamma</t>
-  </si>
-  <si>
-    <t>GAMMA</t>
-  </si>
-  <si>
-    <t>F-Cp</t>
-  </si>
-  <si>
-    <t>FCp</t>
-  </si>
-  <si>
-    <t>F-gamma</t>
-  </si>
-  <si>
-    <t>FGAMMA</t>
-  </si>
-  <si>
-    <t>F-h</t>
-  </si>
-  <si>
-    <t>Fh</t>
-  </si>
-  <si>
-    <t>IF</t>
-  </si>
-  <si>
-    <t>SIF</t>
-  </si>
-  <si>
-    <t>CPSIF</t>
-  </si>
-  <si>
-    <t>Area*</t>
-  </si>
-  <si>
-    <t>AREA</t>
-  </si>
-  <si>
-    <t>Hfp*</t>
-  </si>
-  <si>
-    <t>HFP</t>
-  </si>
-  <si>
-    <t>Rhou*</t>
-  </si>
-  <si>
-    <t>RHOU</t>
-  </si>
-  <si>
-    <t>Hwall*</t>
-  </si>
-  <si>
-    <t>HWALL</t>
-  </si>
-  <si>
-    <t>Qntu*</t>
-  </si>
-  <si>
-    <t>QNTU</t>
-  </si>
-  <si>
     <t>Qpack*</t>
   </si>
   <si>
@@ -284,12 +200,6 @@
     <t>DB</t>
   </si>
   <si>
-    <t>Qreact*</t>
-  </si>
-  <si>
-    <t>QREACT</t>
-  </si>
-  <si>
     <t>H2O</t>
   </si>
   <si>
@@ -368,25 +278,58 @@
     <t>burn_distance_units</t>
   </si>
   <si>
+    <t>Mdotout*</t>
+  </si>
+  <si>
+    <t>filter_temperatures</t>
+  </si>
+  <si>
+    <t>filter_temperature_units</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>filter_absorption_rates</t>
+  </si>
+  <si>
+    <t>filter_absorption_rate_units</t>
+  </si>
+  <si>
+    <t>TPACK</t>
+  </si>
+  <si>
+    <t>wall_left_temperatures</t>
+  </si>
+  <si>
+    <t>wall_temperature_units</t>
+  </si>
+  <si>
+    <t>wall_left_heats</t>
+  </si>
+  <si>
     <t>wall_heat_units</t>
   </si>
   <si>
-    <t>Mdotout*</t>
-  </si>
-  <si>
-    <t>wall_left_temperatures</t>
-  </si>
-  <si>
-    <t>wall_temperature_units</t>
-  </si>
-  <si>
-    <t>wall_left_heats</t>
+    <t>filter_energies</t>
+  </si>
+  <si>
+    <t>filter_energy_units</t>
   </si>
   <si>
     <t>wall_energies</t>
   </si>
   <si>
     <t>wall_energy_units</t>
+  </si>
+  <si>
+    <t>exit_gas_temperatures</t>
+  </si>
+  <si>
+    <t>exit_gas_temperature_units</t>
+  </si>
+  <si>
+    <t>EGT</t>
   </si>
 </sst>
 </file>
@@ -1263,11 +1206,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1307,7 +1250,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
@@ -1324,7 +1267,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
@@ -1356,7 +1299,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>18</v>
@@ -1367,593 +1310,346 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="3" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E14" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E15" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="E16" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="E17" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E18" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="E19" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="E20" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1986,61 +1682,61 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="B11" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fixed logic in orifice parsing
</commit_message>
<xml_diff>
--- a/MappingConfigFile.xlsx
+++ b/MappingConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AIPP3ScilabConvertCompare\GIT\AIPP_scilab_Convert_Compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF0B4E9-3CC5-4FF1-AD22-0F79D42215CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33F185D-FDA8-4916-90EA-3B6A2B49365E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31875" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29715" yWindow="915" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MappingTable" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
   <si>
     <t>AIPP 2.3.5</t>
   </si>
@@ -1210,7 +1210,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,7 +1316,7 @@
         <v>94</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>95</v>

</xml_diff>